<commit_message>
Add 5 and 6
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -5,17 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThetNaungHset\Desktop\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThetNaungHset\Desktop\Kotoba\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="5" r:id="rId1"/>
     <sheet name="Data2" sheetId="2" r:id="rId2"/>
     <sheet name="Data3" sheetId="3" r:id="rId3"/>
     <sheet name="Data4" sheetId="4" r:id="rId4"/>
+    <sheet name="Data5" sheetId="6" r:id="rId5"/>
+    <sheet name="Data6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="499">
   <si>
     <t>わたし</t>
   </si>
@@ -1161,6 +1163,369 @@
   </si>
   <si>
     <t>အနုပညာပြတိုက်အမည်</t>
+  </si>
+  <si>
+    <t>いきます</t>
+  </si>
+  <si>
+    <t>သွားသည်</t>
+  </si>
+  <si>
+    <t>きます</t>
+  </si>
+  <si>
+    <t>လာသည်</t>
+  </si>
+  <si>
+    <t>かえります</t>
+  </si>
+  <si>
+    <t>ပြန်သည်</t>
+  </si>
+  <si>
+    <t>がっこう</t>
+  </si>
+  <si>
+    <t>ကျောင်း</t>
+  </si>
+  <si>
+    <t>スーパー</t>
+  </si>
+  <si>
+    <t>စူပါမားကတ်</t>
+  </si>
+  <si>
+    <t>えき</t>
+  </si>
+  <si>
+    <t>ဘူတာ</t>
+  </si>
+  <si>
+    <t>ひこうき</t>
+  </si>
+  <si>
+    <t>လေယာဥ်ပျံ</t>
+  </si>
+  <si>
+    <t>ふね</t>
+  </si>
+  <si>
+    <t>သင်္ဘော</t>
+  </si>
+  <si>
+    <t>でんしゃ</t>
+  </si>
+  <si>
+    <t>ရထား</t>
+  </si>
+  <si>
+    <t>ちかてつ</t>
+  </si>
+  <si>
+    <t>မြေအောက်ရထား</t>
+  </si>
+  <si>
+    <t>しんかんせん</t>
+  </si>
+  <si>
+    <t>ကျည်ဆန်ရထား</t>
+  </si>
+  <si>
+    <t>バス</t>
+  </si>
+  <si>
+    <t>ဘတ်စ်ကား</t>
+  </si>
+  <si>
+    <t>タクシー</t>
+  </si>
+  <si>
+    <t>တက္ကစီ</t>
+  </si>
+  <si>
+    <t>じてんしゃ</t>
+  </si>
+  <si>
+    <t>စက်ဘီး</t>
+  </si>
+  <si>
+    <t>あるいて</t>
+  </si>
+  <si>
+    <t>လမ်းလျှောက်ပြီး</t>
+  </si>
+  <si>
+    <t>ひと</t>
+  </si>
+  <si>
+    <t>လူ</t>
+  </si>
+  <si>
+    <t>ともだち</t>
+  </si>
+  <si>
+    <t>သူငယ်ချင်း</t>
+  </si>
+  <si>
+    <t>かれ</t>
+  </si>
+  <si>
+    <t>သူ၊ ယောကျ်ားလေး သူငယ်ချင်း (ရည်းစား)</t>
+  </si>
+  <si>
+    <t>かのじょ</t>
+  </si>
+  <si>
+    <t>သူမ၊ မိန်းကလေး သူငယ်ချင်း (ရည်းစား)</t>
+  </si>
+  <si>
+    <t>かぞく</t>
+  </si>
+  <si>
+    <t>မိသားစု</t>
+  </si>
+  <si>
+    <t>ひとりで</t>
+  </si>
+  <si>
+    <t>တစ်ယောက်တည်း</t>
+  </si>
+  <si>
+    <t>せんしゅう</t>
+  </si>
+  <si>
+    <t>ပြီးခဲ့တဲ့အပတ်</t>
+  </si>
+  <si>
+    <t>こんしゅう</t>
+  </si>
+  <si>
+    <t>ဒီအပတ်</t>
+  </si>
+  <si>
+    <t>らいしゅう</t>
+  </si>
+  <si>
+    <t>လာမည့်အပတ်၊  နောက်အပတ်</t>
+  </si>
+  <si>
+    <t>せんげつ</t>
+  </si>
+  <si>
+    <t>ပြီးခဲ့တဲ့လ</t>
+  </si>
+  <si>
+    <t>こんげつ</t>
+  </si>
+  <si>
+    <t>ဒီလ</t>
+  </si>
+  <si>
+    <t>らいげつ</t>
+  </si>
+  <si>
+    <t>လာမည့်လ၊ နောက်လ</t>
+  </si>
+  <si>
+    <t>きょねん</t>
+  </si>
+  <si>
+    <t>ပြီးခဲ့တဲ့နှစ်၊ မနှစ်က</t>
+  </si>
+  <si>
+    <t>ことし</t>
+  </si>
+  <si>
+    <t>ဒီနှစ်</t>
+  </si>
+  <si>
+    <t>らいねん</t>
+  </si>
+  <si>
+    <t>လာမည့်နှစ်၊ နောက်နှစ်</t>
+  </si>
+  <si>
+    <t>ーねん</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - နှစ်</t>
+  </si>
+  <si>
+    <t>なんねん</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ဘယ်နှစ်</t>
+  </si>
+  <si>
+    <t>ーがつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - လ</t>
+  </si>
+  <si>
+    <t>なんがつ</t>
+  </si>
+  <si>
+    <t>ဘယ်လ</t>
+  </si>
+  <si>
+    <t>ついたち</t>
+  </si>
+  <si>
+    <t>၁ ရက်နေ့၊ ၁ ရက်</t>
+  </si>
+  <si>
+    <t>ふつか</t>
+  </si>
+  <si>
+    <t>၂ ရက်နေ့၊ ၂ ရက်</t>
+  </si>
+  <si>
+    <t>みっか</t>
+  </si>
+  <si>
+    <t>၃ ရက်နေ့၊ ၃ ရက်</t>
+  </si>
+  <si>
+    <t>よっか</t>
+  </si>
+  <si>
+    <t>၄ ရက်နေ့၊ ၄ ရက်</t>
+  </si>
+  <si>
+    <t>いつか</t>
+  </si>
+  <si>
+    <t>၅ ရက်နေ့၊ ၅ ရက်</t>
+  </si>
+  <si>
+    <t>むいか</t>
+  </si>
+  <si>
+    <t>၆ ရက်နေ့၊ ၆ ရက်</t>
+  </si>
+  <si>
+    <t>なのか</t>
+  </si>
+  <si>
+    <t>၇ ရက်နေ့၊ ၇ ရက်</t>
+  </si>
+  <si>
+    <t>ようか</t>
+  </si>
+  <si>
+    <t>၈ ရက်နေ့၊ ၈ ရက်</t>
+  </si>
+  <si>
+    <t>ここのか</t>
+  </si>
+  <si>
+    <t>၉ ရက်နေ့၊ ၉ ရက်</t>
+  </si>
+  <si>
+    <t>とおか</t>
+  </si>
+  <si>
+    <t>၁၀ ရက်နေ့၊ ၁၀ ရက်</t>
+  </si>
+  <si>
+    <t>じゅうよっか</t>
+  </si>
+  <si>
+    <t>၁၄ ရက်နေ့၊ ၁၄ ရက်</t>
+  </si>
+  <si>
+    <t>はつか</t>
+  </si>
+  <si>
+    <t>၂၀ ရက်နေ့၊ ၂၀ ရက်</t>
+  </si>
+  <si>
+    <t>にじゅうよっか</t>
+  </si>
+  <si>
+    <t>၂၄ ရက်နေ့၊ ၂၄ ရက်</t>
+  </si>
+  <si>
+    <t>ーにち</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ရက်နေ့၊ - ရက်</t>
+  </si>
+  <si>
+    <t>なんにち</t>
+  </si>
+  <si>
+    <t>ဘယ်ရက်နေ့၊ ဘယ်ရက်</t>
+  </si>
+  <si>
+    <t>いつ</t>
+  </si>
+  <si>
+    <t>ဘယ်အချိန်၊ ဘယ်တော့</t>
+  </si>
+  <si>
+    <t>たんじょうび</t>
+  </si>
+  <si>
+    <t>မွေးနေ့</t>
+  </si>
+  <si>
+    <t>そうですね</t>
+  </si>
+  <si>
+    <t>ဟုတ်တယ်နော်</t>
+  </si>
+  <si>
+    <t>「どうも」ありがとう　ございました</t>
+  </si>
+  <si>
+    <t>どう　いたしまして</t>
+  </si>
+  <si>
+    <t>မဟုတ်တာ၊ ရပါတယ်</t>
+  </si>
+  <si>
+    <t>ーばんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - စင်္ကြန်</t>
+  </si>
+  <si>
+    <t>つぎの</t>
+  </si>
+  <si>
+    <t>နောက်လာမည့်</t>
+  </si>
+  <si>
+    <t>ふつう</t>
+  </si>
+  <si>
+    <t>ရိုးရိုး (ရထားအမျိုးအစား)</t>
+  </si>
+  <si>
+    <t>きゅうこう</t>
+  </si>
+  <si>
+    <t>အမြန် (ရထားအမျိုးအစား)</t>
+  </si>
+  <si>
+    <t>とっきゅう</t>
+  </si>
+  <si>
+    <t>အထူးအမြန် (ရထားအမျိုးအစား)</t>
+  </si>
+  <si>
+    <t>こうしえん</t>
+  </si>
+  <si>
+    <t>ခိုးရှိအမ်း</t>
+  </si>
+  <si>
+    <t>おおさかじょう</t>
+  </si>
+  <si>
+    <t>အိုဆာကာရဲတိုက်</t>
   </si>
 </sst>
 </file>
@@ -1567,7 +1932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -2361,7 +2726,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -2460,7 +2825,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -2653,7 +3018,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2675,7 +3040,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2686,7 +3051,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2719,7 +3084,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2741,7 +3106,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2752,7 +3117,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2763,7 +3128,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2785,7 +3150,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2851,7 +3216,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2873,7 +3238,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2884,7 +3249,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2895,7 +3260,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2906,7 +3271,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2928,7 +3293,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -2939,7 +3304,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2950,7 +3315,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -2961,7 +3326,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -2972,7 +3337,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -2983,7 +3348,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3005,7 +3370,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -3060,7 +3425,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -3082,7 +3447,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -3109,7 +3474,7 @@
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3128,7 +3493,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3150,7 +3515,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3161,7 +3526,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3172,7 +3537,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3227,7 +3592,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3238,7 +3603,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3271,7 +3636,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3293,7 +3658,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3304,7 +3669,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3315,7 +3680,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3326,7 +3691,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3348,7 +3713,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3403,7 +3768,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3425,7 +3790,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3447,7 +3812,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -3458,7 +3823,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3480,7 +3845,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -3568,7 +3933,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -3579,7 +3944,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -3612,7 +3977,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -3656,7 +4021,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -3678,7 +4043,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -3700,7 +4065,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -3722,7 +4087,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -3744,7 +4109,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -3755,7 +4120,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -3766,7 +4131,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -3786,6 +4151,1404 @@
       </c>
       <c r="C61" s="8" t="s">
         <v>377</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="78" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="51" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="78" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
L 11 to 13
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="668" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="668" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="5" r:id="rId1"/>
@@ -22,24 +22,27 @@
     <sheet name="Data8" sheetId="12" r:id="rId8"/>
     <sheet name="Data9" sheetId="28" r:id="rId9"/>
     <sheet name="Data10" sheetId="29" r:id="rId10"/>
-    <sheet name="Verb" sheetId="9" r:id="rId11"/>
-    <sheet name="Bonpoe1" sheetId="10" r:id="rId12"/>
-    <sheet name="Bonpoe2" sheetId="14" r:id="rId13"/>
-    <sheet name="Bonpoe3" sheetId="15" r:id="rId14"/>
-    <sheet name="Bonpoe4" sheetId="16" r:id="rId15"/>
-    <sheet name="Bonpoe5" sheetId="17" r:id="rId16"/>
-    <sheet name="Bonpoe6" sheetId="19" r:id="rId17"/>
-    <sheet name="Bonpoe7" sheetId="18" r:id="rId18"/>
-    <sheet name="hiragana" sheetId="20" r:id="rId19"/>
-    <sheet name="dakuon" sheetId="22" r:id="rId20"/>
-    <sheet name="handakuon" sheetId="23" r:id="rId21"/>
-    <sheet name="youon" sheetId="24" r:id="rId22"/>
-    <sheet name="katakana" sheetId="21" r:id="rId23"/>
-    <sheet name="kdakuon" sheetId="25" r:id="rId24"/>
-    <sheet name="khandakuon" sheetId="26" r:id="rId25"/>
-    <sheet name="kyouon" sheetId="27" r:id="rId26"/>
-    <sheet name="Sheet1" sheetId="13" r:id="rId27"/>
-    <sheet name="Q" sheetId="11" r:id="rId28"/>
+    <sheet name="Data11" sheetId="32" r:id="rId11"/>
+    <sheet name="Data12" sheetId="31" r:id="rId12"/>
+    <sheet name="Data13" sheetId="30" r:id="rId13"/>
+    <sheet name="Verb" sheetId="9" r:id="rId14"/>
+    <sheet name="Bonpoe1" sheetId="10" r:id="rId15"/>
+    <sheet name="Bonpoe2" sheetId="14" r:id="rId16"/>
+    <sheet name="Bonpoe3" sheetId="15" r:id="rId17"/>
+    <sheet name="Bonpoe4" sheetId="16" r:id="rId18"/>
+    <sheet name="Bonpoe5" sheetId="17" r:id="rId19"/>
+    <sheet name="Bonpoe6" sheetId="19" r:id="rId20"/>
+    <sheet name="Bonpoe7" sheetId="18" r:id="rId21"/>
+    <sheet name="hiragana" sheetId="20" r:id="rId22"/>
+    <sheet name="dakuon" sheetId="22" r:id="rId23"/>
+    <sheet name="handakuon" sheetId="23" r:id="rId24"/>
+    <sheet name="youon" sheetId="24" r:id="rId25"/>
+    <sheet name="katakana" sheetId="21" r:id="rId26"/>
+    <sheet name="kdakuon" sheetId="25" r:id="rId27"/>
+    <sheet name="khandakuon" sheetId="26" r:id="rId28"/>
+    <sheet name="kyouon" sheetId="27" r:id="rId29"/>
+    <sheet name="Sheet1" sheetId="13" r:id="rId30"/>
+    <sheet name="Q" sheetId="11" r:id="rId31"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -51,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1633">
   <si>
     <t>わたし</t>
   </si>
@@ -4305,6 +4308,870 @@
   </si>
   <si>
     <t>びじゅつかん</t>
+  </si>
+  <si>
+    <t>います「こどもが～」</t>
+  </si>
+  <si>
+    <t>ရှိသည် [ကလေး~]</t>
+  </si>
+  <si>
+    <t>います「にほんに～」</t>
+  </si>
+  <si>
+    <t>ရှိသည် [ဂျပန်မှာ~]</t>
+  </si>
+  <si>
+    <t>かかります</t>
+  </si>
+  <si>
+    <t>ကြာသည်၊ ကုန်ကျသည်</t>
+  </si>
+  <si>
+    <t>やすみます「かいしゃを～」</t>
+  </si>
+  <si>
+    <t>နားသည်၊ အနားယူသည်</t>
+  </si>
+  <si>
+    <t>ひとつ</t>
+  </si>
+  <si>
+    <t>တစ်ခု</t>
+  </si>
+  <si>
+    <t>ふたつ</t>
+  </si>
+  <si>
+    <t>နှစ်ခု</t>
+  </si>
+  <si>
+    <t>みっつ</t>
+  </si>
+  <si>
+    <t>သုံးခု</t>
+  </si>
+  <si>
+    <t>よっつ</t>
+  </si>
+  <si>
+    <t>လေးခု</t>
+  </si>
+  <si>
+    <t>いつつ</t>
+  </si>
+  <si>
+    <t>ငါးခု</t>
+  </si>
+  <si>
+    <t>むっつ</t>
+  </si>
+  <si>
+    <t>ခြောက်ခု</t>
+  </si>
+  <si>
+    <t>ななつ</t>
+  </si>
+  <si>
+    <t>ခုနှစ်ခု</t>
+  </si>
+  <si>
+    <t>やっつ</t>
+  </si>
+  <si>
+    <t>ရှစ်ခု</t>
+  </si>
+  <si>
+    <t>ここのつ</t>
+  </si>
+  <si>
+    <t>ကိုးခု</t>
+  </si>
+  <si>
+    <t>とお</t>
+  </si>
+  <si>
+    <t>ဆယ်ခု</t>
+  </si>
+  <si>
+    <t>いくつ</t>
+  </si>
+  <si>
+    <t>ဘယ်နှစ်ခု</t>
+  </si>
+  <si>
+    <t>ひとり</t>
+  </si>
+  <si>
+    <t>တစ်ယောက်၊ တစ်ဦး</t>
+  </si>
+  <si>
+    <t>ふたり</t>
+  </si>
+  <si>
+    <t>နှစ်ယောက်၊ နှစ်ဦး</t>
+  </si>
+  <si>
+    <t>ーにん</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ယောက်၊ - ဦး</t>
+  </si>
+  <si>
+    <t>ーだい</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - လုံး၊ - စီး</t>
+  </si>
+  <si>
+    <t>ーまい</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ချပ်၊ ရွက်</t>
+  </si>
+  <si>
+    <t>ーかい</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ကြိမ်၊ - ခါ</t>
+  </si>
+  <si>
+    <t>りんご</t>
+  </si>
+  <si>
+    <t>ပန်းသီး</t>
+  </si>
+  <si>
+    <t>みかん</t>
+  </si>
+  <si>
+    <t>လိမ္မော်သီး</t>
+  </si>
+  <si>
+    <t>サンドイッチ</t>
+  </si>
+  <si>
+    <t>ဆန်းဒွစ်ချ်</t>
+  </si>
+  <si>
+    <t>カレー「ライス」</t>
+  </si>
+  <si>
+    <t>မဆလာဟင်း၊ ကာရီ [ထမင်း]</t>
+  </si>
+  <si>
+    <t>アイスクリーム</t>
+  </si>
+  <si>
+    <t>ရေခဲမုန့်</t>
+  </si>
+  <si>
+    <t>きって</t>
+  </si>
+  <si>
+    <t>တံဆိပ်ခေါင်း</t>
+  </si>
+  <si>
+    <t>はがき</t>
+  </si>
+  <si>
+    <t>ပို့စကတ်</t>
+  </si>
+  <si>
+    <t>ふうとう</t>
+  </si>
+  <si>
+    <t>စာအိတ်</t>
+  </si>
+  <si>
+    <t>りょうしん</t>
+  </si>
+  <si>
+    <t>မိဘ</t>
+  </si>
+  <si>
+    <t>きょうだい</t>
+  </si>
+  <si>
+    <t>ညီအစ်ကို၊ မောင်နှမ</t>
+  </si>
+  <si>
+    <t>あに</t>
+  </si>
+  <si>
+    <t>အစ်ကို (မိမိ၏~)</t>
+  </si>
+  <si>
+    <t>おにいさん</t>
+  </si>
+  <si>
+    <t>အစ်ကို (တစ်ပါးသူ၏~)</t>
+  </si>
+  <si>
+    <t>あね</t>
+  </si>
+  <si>
+    <t>အစ်မ (မိမိ၏~)</t>
+  </si>
+  <si>
+    <t>おねえさん</t>
+  </si>
+  <si>
+    <t>အစ်မ (တစ်ပါးသူ၏~)</t>
+  </si>
+  <si>
+    <t>おとうと</t>
+  </si>
+  <si>
+    <t>ညီ၊ မောင် (မိမိ၏~)</t>
+  </si>
+  <si>
+    <t>おとうとさん</t>
+  </si>
+  <si>
+    <t>ညီ၊ မောင် (တစ်ပါးသူ၏~)</t>
+  </si>
+  <si>
+    <t>いもうと</t>
+  </si>
+  <si>
+    <t>ညီမ၊ နှမ (မိမိ၏~)</t>
+  </si>
+  <si>
+    <t>いもうとさん</t>
+  </si>
+  <si>
+    <t>ညီမ၊ နှမ (တစ်ပါးသူ၏~)</t>
+  </si>
+  <si>
+    <t>がいこく</t>
+  </si>
+  <si>
+    <t>နိုင်ငံခြား၊ ပြည်ပ</t>
+  </si>
+  <si>
+    <t>りゅうがくせい</t>
+  </si>
+  <si>
+    <t>နိုင်ငံခြားပညာသင် ကျောင်းသား</t>
+  </si>
+  <si>
+    <t>クラス</t>
+  </si>
+  <si>
+    <t>အတန်း</t>
+  </si>
+  <si>
+    <t>ーじかん</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - နာရီကြာ</t>
+  </si>
+  <si>
+    <t>ーしゅうかん</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ပတ်ကြာ</t>
+  </si>
+  <si>
+    <t>ーかげつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - လကြာ</t>
+  </si>
+  <si>
+    <t>～ぐらい</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ လောက်၊ ~ ခန့်</t>
+  </si>
+  <si>
+    <t>どのぐらい</t>
+  </si>
+  <si>
+    <t>ဘယ်လောက်ကြာကြာ၊ ဘယ်လောက်လောက်</t>
+  </si>
+  <si>
+    <t>ぜんぶで</t>
+  </si>
+  <si>
+    <t>အားလုံးပေါင်း၊ စုစုပေါင်း</t>
+  </si>
+  <si>
+    <t>みんな</t>
+  </si>
+  <si>
+    <t>အားလုံး</t>
+  </si>
+  <si>
+    <t>～だけ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ သာ၊ ~ တည်းသာ</t>
+  </si>
+  <si>
+    <t>かしこまりました</t>
+  </si>
+  <si>
+    <t>いい「お」てんきですね</t>
+  </si>
+  <si>
+    <t>ရာသီဥတုသာယာတယ်နော်</t>
+  </si>
+  <si>
+    <t>おでかけですか</t>
+  </si>
+  <si>
+    <t>အပြင်ထွက်မလို့လား</t>
+  </si>
+  <si>
+    <t>ちょっと　～まで</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ နားလေးတင်</t>
+  </si>
+  <si>
+    <t>いってらっしゃい</t>
+  </si>
+  <si>
+    <t>ကောင်းကောင်းသွားနော်</t>
+  </si>
+  <si>
+    <t>いってきます</t>
+  </si>
+  <si>
+    <t>သွားပြီနော်</t>
+  </si>
+  <si>
+    <t>ふなびん</t>
+  </si>
+  <si>
+    <t>ရေကြောင်းစာ၊ ဆီးမေးလ်</t>
+  </si>
+  <si>
+    <t>こうくうびん（エアメール）</t>
+  </si>
+  <si>
+    <t>လေကြောင်းစာ၊ အဲယားမေးလ်</t>
+  </si>
+  <si>
+    <t>おねがいします</t>
+  </si>
+  <si>
+    <t>ဆောင်ရွက်ပေးပါ၊ ကူညီပေးပါ</t>
+  </si>
+  <si>
+    <t>オーストラリア</t>
+  </si>
+  <si>
+    <t>သြစတြေးလျ</t>
+  </si>
+  <si>
+    <t>かんたん「な」</t>
+  </si>
+  <si>
+    <t>လွယ်ကူသော၊ ရိုးရှင်းသော</t>
+  </si>
+  <si>
+    <t>ちかい</t>
+  </si>
+  <si>
+    <t>နီးသော</t>
+  </si>
+  <si>
+    <t>とおい</t>
+  </si>
+  <si>
+    <t>ဝေးသော</t>
+  </si>
+  <si>
+    <t>はやい</t>
+  </si>
+  <si>
+    <t>မြန်သော၊ စောသော</t>
+  </si>
+  <si>
+    <t>おそい</t>
+  </si>
+  <si>
+    <t>နှေးသော၊ နောက်ကျသော</t>
+  </si>
+  <si>
+    <t>おおい「ひとが～」</t>
+  </si>
+  <si>
+    <t>များသော [ လူက ~ ]</t>
+  </si>
+  <si>
+    <t>すくない「ひとが～」</t>
+  </si>
+  <si>
+    <t>နည်းသော [ လူက ~ ]</t>
+  </si>
+  <si>
+    <t>あたたかい</t>
+  </si>
+  <si>
+    <t>နွေးသော၊ နွေးထွေးသော</t>
+  </si>
+  <si>
+    <t>すずしい</t>
+  </si>
+  <si>
+    <t>အေးမြသော</t>
+  </si>
+  <si>
+    <t>あまい</t>
+  </si>
+  <si>
+    <t>ချိုသော</t>
+  </si>
+  <si>
+    <t>からい</t>
+  </si>
+  <si>
+    <t>စပ်သော</t>
+  </si>
+  <si>
+    <t>おもい</t>
+  </si>
+  <si>
+    <t>လေးသော</t>
+  </si>
+  <si>
+    <t>かるい</t>
+  </si>
+  <si>
+    <t>ပေါ့သော</t>
+  </si>
+  <si>
+    <t>いい「コーヒーが～」</t>
+  </si>
+  <si>
+    <t>ကောင်းတယ်</t>
+  </si>
+  <si>
+    <t>きせつ</t>
+  </si>
+  <si>
+    <t>ရာသီ ဥတု</t>
+  </si>
+  <si>
+    <t>はる</t>
+  </si>
+  <si>
+    <t>နွေဦး</t>
+  </si>
+  <si>
+    <t>なつ</t>
+  </si>
+  <si>
+    <t>နွေ</t>
+  </si>
+  <si>
+    <t>あき</t>
+  </si>
+  <si>
+    <t>ဆောင်းဦး</t>
+  </si>
+  <si>
+    <t>ふゆ</t>
+  </si>
+  <si>
+    <t>ဆောင်း</t>
+  </si>
+  <si>
+    <t>てんき</t>
+  </si>
+  <si>
+    <t>မိုးလေဝသ</t>
+  </si>
+  <si>
+    <t>あめ</t>
+  </si>
+  <si>
+    <t>မိုး၊ မိုးရွာသော</t>
+  </si>
+  <si>
+    <t>ゆき</t>
+  </si>
+  <si>
+    <t>နှင်း၊ နှင်းကျသော</t>
+  </si>
+  <si>
+    <t>くもり</t>
+  </si>
+  <si>
+    <t>မိုးအုံ့သော၊ တိမ်ထူသော</t>
+  </si>
+  <si>
+    <t>ホテル</t>
+  </si>
+  <si>
+    <t>ဟိုတယ်</t>
+  </si>
+  <si>
+    <t>くうこう</t>
+  </si>
+  <si>
+    <t>လေဆိပ်၊ လေယာဥ်ကွင်း</t>
+  </si>
+  <si>
+    <t>うみ</t>
+  </si>
+  <si>
+    <t>ပင်လယ်</t>
+  </si>
+  <si>
+    <t>せかい</t>
+  </si>
+  <si>
+    <t>ကမ္ဘာ</t>
+  </si>
+  <si>
+    <t>パーティー</t>
+  </si>
+  <si>
+    <t>ပါတီ</t>
+  </si>
+  <si>
+    <t>「お」まつり</t>
+  </si>
+  <si>
+    <t>ပွဲ</t>
+  </si>
+  <si>
+    <t>すきやき</t>
+  </si>
+  <si>
+    <t>စူခိရခိ</t>
+  </si>
+  <si>
+    <t>さしみ</t>
+  </si>
+  <si>
+    <t>ဆာရှိမိ၊ ငါးစိမ်းလွှာ</t>
+  </si>
+  <si>
+    <t>「お」すし</t>
+  </si>
+  <si>
+    <t>ဆူရှီ</t>
+  </si>
+  <si>
+    <t>てんぷら</t>
+  </si>
+  <si>
+    <t>တန်ပူရာ</t>
+  </si>
+  <si>
+    <t>ぶたにく</t>
+  </si>
+  <si>
+    <t>ဝက်သား</t>
+  </si>
+  <si>
+    <t>とりにく</t>
+  </si>
+  <si>
+    <t>ကြက်သား</t>
+  </si>
+  <si>
+    <t>ぎゅうにく</t>
+  </si>
+  <si>
+    <t>အမဲသား</t>
+  </si>
+  <si>
+    <t>レモン</t>
+  </si>
+  <si>
+    <t>သံပရို၊ လီမွန်</t>
+  </si>
+  <si>
+    <t>いけばな</t>
+  </si>
+  <si>
+    <t>အိခဲဘန၊ ဂျပန်ရိုးရာ ပန်းအလှ</t>
+  </si>
+  <si>
+    <t>もみじ</t>
+  </si>
+  <si>
+    <t>မိုးမိဂျိ၊ မေပယ်ရွက်</t>
+  </si>
+  <si>
+    <t>ဘယ်တစ်ခု</t>
+  </si>
+  <si>
+    <t>どちらも</t>
+  </si>
+  <si>
+    <t>နှစ်ခုစလုံး၊ ဘယ်ဟာဖြစ်ဖြစ်</t>
+  </si>
+  <si>
+    <t>いちばん</t>
+  </si>
+  <si>
+    <t>ပထမ၊ အကြိုက်ဆုံး</t>
+  </si>
+  <si>
+    <t>ずっと</t>
+  </si>
+  <si>
+    <t>အပြတ်အသတ်၊ သိသိသာသာ</t>
+  </si>
+  <si>
+    <t>はじめて</t>
+  </si>
+  <si>
+    <t>ပထမဦးဆုံး</t>
+  </si>
+  <si>
+    <t>ただいま</t>
+  </si>
+  <si>
+    <t>ပြန်ရောက်ပါပြီ</t>
+  </si>
+  <si>
+    <t>おかえりなさい</t>
+  </si>
+  <si>
+    <t>ပြန်လာပြီလား</t>
+  </si>
+  <si>
+    <t>わあ、すごい　ひとですね</t>
+  </si>
+  <si>
+    <t>ဟယ်... လူတော်တော်စည်တယ်နော်</t>
+  </si>
+  <si>
+    <t>つかれました</t>
+  </si>
+  <si>
+    <t>ပင်ပန်းတယ်၊ ပင်ပန်းသွားပြီ</t>
+  </si>
+  <si>
+    <t>ぎおんまつり</t>
+  </si>
+  <si>
+    <t>ဂိအွန်းပွဲတော်</t>
+  </si>
+  <si>
+    <t>ホンコン</t>
+  </si>
+  <si>
+    <t>ဟောင်ကောင်</t>
+  </si>
+  <si>
+    <t>シンガポール</t>
+  </si>
+  <si>
+    <t>စင်္ကာပူ</t>
+  </si>
+  <si>
+    <t>ABC ストア</t>
+  </si>
+  <si>
+    <t>ジャパン</t>
+  </si>
+  <si>
+    <t>あそびます</t>
+  </si>
+  <si>
+    <t>လျှောက်လည်သည်၊ လည်ပတ်သည်၊ ကစားသည်</t>
+  </si>
+  <si>
+    <t>およぎます</t>
+  </si>
+  <si>
+    <t>ရေကူးသည်</t>
+  </si>
+  <si>
+    <t>むかえます</t>
+  </si>
+  <si>
+    <t>ကြိုဆိုသည်</t>
+  </si>
+  <si>
+    <t>つかれます</t>
+  </si>
+  <si>
+    <t>ပင်ပန်းသည်</t>
+  </si>
+  <si>
+    <t>けっこんします</t>
+  </si>
+  <si>
+    <t>လက်ထပ်သည်၊ မင်္ဂလာဆောင်သည်</t>
+  </si>
+  <si>
+    <t>かいものします</t>
+  </si>
+  <si>
+    <t>စျေးဝယ်သည်</t>
+  </si>
+  <si>
+    <t>しょくじします</t>
+  </si>
+  <si>
+    <t>ထမင်းစားသည်၊ စားသောက်သည်</t>
+  </si>
+  <si>
+    <t>さんぽします「こうえんを～」</t>
+  </si>
+  <si>
+    <t>လမ်းလျှောက်သည်</t>
+  </si>
+  <si>
+    <t>たいへん「な」</t>
+  </si>
+  <si>
+    <t>ဒုက္ခကြီးသော၊ မလွယ်လှသော</t>
+  </si>
+  <si>
+    <t>ほしい</t>
+  </si>
+  <si>
+    <t>လိုချင်သော၊ တပ်မက်သော</t>
+  </si>
+  <si>
+    <t>ひろい</t>
+  </si>
+  <si>
+    <t>ကျယ်ဝန်းသော</t>
+  </si>
+  <si>
+    <t>せまい</t>
+  </si>
+  <si>
+    <t>ကျဥ်းမြောင်းသော</t>
+  </si>
+  <si>
+    <t>プール</t>
+  </si>
+  <si>
+    <t>ရေကူးကန်</t>
+  </si>
+  <si>
+    <t>かわ</t>
+  </si>
+  <si>
+    <t>မြစ်၊ ချောင်း</t>
+  </si>
+  <si>
+    <t>びじゅつ</t>
+  </si>
+  <si>
+    <t>အနုပညာ</t>
+  </si>
+  <si>
+    <t>つり</t>
+  </si>
+  <si>
+    <t>ငါးမျှားခြင်း</t>
+  </si>
+  <si>
+    <t>スキー</t>
+  </si>
+  <si>
+    <t>စကီး၊ နှင်းလျှော</t>
+  </si>
+  <si>
+    <t>しゅうまつ</t>
+  </si>
+  <si>
+    <t>စနေ၊ တနင်္ဂနွေ</t>
+  </si>
+  <si>
+    <t>「お」しょうがつ</t>
+  </si>
+  <si>
+    <t>နှစ်သစ်ကူး</t>
+  </si>
+  <si>
+    <t>～ごろ</t>
+  </si>
+  <si>
+    <t>~ လောက်၊ ~ ဝန်းကျင်</t>
+  </si>
+  <si>
+    <t>なにか</t>
+  </si>
+  <si>
+    <t>တစ်ခုခု</t>
+  </si>
+  <si>
+    <t>どこか</t>
+  </si>
+  <si>
+    <t>တစ်နေရာရာ</t>
+  </si>
+  <si>
+    <t>のどが　かわきます</t>
+  </si>
+  <si>
+    <t>ရေဆာသည်၊ အာခေါင်ခြောက်သည်</t>
+  </si>
+  <si>
+    <t>おなかが　すきます</t>
+  </si>
+  <si>
+    <t>ဗိုက်ဆာသည်</t>
+  </si>
+  <si>
+    <t>そう　しましょう</t>
+  </si>
+  <si>
+    <t>အဲဒီလိုပဲ လုပ်ကြတာပေါ့</t>
+  </si>
+  <si>
+    <t>ごちゅうもんは？</t>
+  </si>
+  <si>
+    <t>ဘာမှာ လိုပါသလဲ</t>
+  </si>
+  <si>
+    <t>ていしょく</t>
+  </si>
+  <si>
+    <t>အမျိုး အမယ် အရေအတွက် သတ်မှတ်ထားသော အစား အသောက်တစ်စုံစာ၊ တစ်ယောက်စာ စားပွဲတစ်စုံ</t>
+  </si>
+  <si>
+    <t>ぎゅうどん</t>
+  </si>
+  <si>
+    <t>အမဲသားဟင်းပုံ ထမင်း</t>
+  </si>
+  <si>
+    <t>「しょうしょう」おまちください</t>
+  </si>
+  <si>
+    <t>[ ခဏလောက် ] စောင့်ပေးပါ</t>
+  </si>
+  <si>
+    <t>～で　ございます</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ~ ဖြစ်ပါတယ်</t>
+  </si>
+  <si>
+    <t>べつべつ</t>
+  </si>
+  <si>
+    <t>သတ်သတ်စီ၊ သီးခြားစီ</t>
+  </si>
+  <si>
+    <t>アキックス</t>
+  </si>
+  <si>
+    <t>ကုမ္ပဏီ အမည်</t>
+  </si>
+  <si>
+    <t>おはよう　テレビ</t>
+  </si>
+  <si>
+    <t>ရုပ်သံလိုင်း အမည်</t>
   </si>
 </sst>
 </file>
@@ -4473,7 +5340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4592,6 +5459,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5311,7 +6182,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5874,6 +6745,1710 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="33"/>
+    <col min="2" max="2" width="40.21875" style="33" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="33" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="41"/>
+    <col min="2" max="2" width="26" style="41" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" style="41" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C28" s="42" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C32" s="42" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C40" s="42" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C43" s="42" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C49" s="42" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C52" s="42" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C53" s="42" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C54" s="42" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.77734375" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="41"/>
+      <c r="B1" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
@@ -6221,7 +8796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
@@ -6437,7 +9012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -6551,7 +9126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -6643,7 +9218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A34"/>
   <sheetViews>
@@ -6798,7 +9373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
@@ -6853,370 +9428,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="79.109375" style="36" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>923</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A18"/>
-  <sheetViews>
-    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="76.21875" style="36" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>928</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="8.88671875" style="38"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>974</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>975</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>976</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>977</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>937</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>938</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>939</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
-        <v>941</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>942</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>943</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>944</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
-        <v>946</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>947</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>948</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>949</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
-        <v>951</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>952</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>953</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>621</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
-        <v>955</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>956</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>957</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>958</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
-        <v>960</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>961</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>962</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>963</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
-        <v>965</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>968</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>969</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>970</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
-        <v>966</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>979</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>967</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>979</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>1029</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>1030</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="38" t="s">
-        <v>979</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>979</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>973</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>979</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>979</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7755,6 +9966,370 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79.109375" style="36" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>923</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="76.21875" style="36" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>928</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.88671875" style="38"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="39" t="s">
+        <v>974</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>975</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>976</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>977</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>937</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>938</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>939</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>941</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>942</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>943</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>944</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
+        <v>946</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>947</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>948</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>949</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
+        <v>951</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>952</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>953</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>621</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>955</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>956</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>957</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>958</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>960</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>961</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>962</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>963</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>965</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>968</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>969</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>970</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>966</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>979</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>967</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>979</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>979</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>979</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>973</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>979</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>979</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
@@ -7856,7 +10431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -7908,7 +10483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -8058,7 +10633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -8280,7 +10855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -8383,7 +10958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -8435,7 +11010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -8579,390 +11154,6 @@
       <c r="C12" s="37" t="s">
         <v>1145</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A34"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="56.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-    </row>
-    <row r="6" spans="1:1" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-    </row>
-    <row r="9" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-    </row>
-    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-    </row>
-    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A16" s="28" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-    </row>
-    <row r="18" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-    </row>
-    <row r="20" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27"/>
-    </row>
-    <row r="24" spans="1:1" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="30" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-    </row>
-    <row r="27" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
-    </row>
-    <row r="29" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
-    </row>
-    <row r="33" spans="1:1" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="30" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
-        <v>701</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="53.33203125" style="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9542,11 +11733,395 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+    </row>
+    <row r="6" spans="1:1" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+    </row>
+    <row r="9" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+    </row>
+    <row r="18" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+    </row>
+    <row r="20" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+    </row>
+    <row r="24" spans="1:1" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="30" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="22"/>
+    </row>
+    <row r="27" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="22"/>
+    </row>
+    <row r="29" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="22" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="22" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="22" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="22"/>
+    </row>
+    <row r="33" spans="1:1" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="30" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
+        <v>701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.33203125" style="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>